<commit_message>
replicate fig 3 of original
</commit_message>
<xml_diff>
--- a/support/replication_details.xlsx
+++ b/support/replication_details.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="1155" yWindow="1785" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="original_country_selection" sheetId="1" r:id="rId1"/>
     <sheet name="code_to_country_lookup" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="replicated_table2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="111">
   <si>
     <t>Country</t>
   </si>
@@ -328,14 +328,53 @@
   </si>
   <si>
     <t>in_original_selection</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>New version</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Original version</t>
+  </si>
+  <si>
+    <t>Proportion difference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -360,14 +399,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -941,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1487,12 +1531,307 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1910</v>
+      </c>
+      <c r="C3" s="1">
+        <v>16.667287240303999</v>
+      </c>
+      <c r="D3" s="1">
+        <v>18.359450211184999</v>
+      </c>
+      <c r="F3">
+        <v>1910</v>
+      </c>
+      <c r="G3">
+        <v>16.760000000000002</v>
+      </c>
+      <c r="H3">
+        <v>18.28</v>
+      </c>
+      <c r="J3" s="2">
+        <f>(G3-C3)/G3</f>
+        <v>5.5317875713605412E-3</v>
+      </c>
+      <c r="K3" s="2">
+        <f>(H3-D3)/H3</f>
+        <v>-4.3462916403171747E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1919</v>
+      </c>
+      <c r="C4" s="1">
+        <v>16.524617064120399</v>
+      </c>
+      <c r="D4" s="1">
+        <v>19.501820872385199</v>
+      </c>
+      <c r="F4">
+        <v>1919</v>
+      </c>
+      <c r="G4">
+        <v>16.440000000000001</v>
+      </c>
+      <c r="H4">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="J4" s="2">
+        <f>(G4-C4)/G4</f>
+        <v>-5.1470233649876882E-3</v>
+      </c>
+      <c r="K4" s="2">
+        <f>(H4-D4)/H4</f>
+        <v>-3.9542690425650187E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1930</v>
+      </c>
+      <c r="C5" s="1">
+        <v>12.873068839654501</v>
+      </c>
+      <c r="D5" s="1">
+        <v>14.489567026066</v>
+      </c>
+      <c r="F5">
+        <v>1930</v>
+      </c>
+      <c r="G5">
+        <v>12.44</v>
+      </c>
+      <c r="H5">
+        <v>13.84</v>
+      </c>
+      <c r="J5" s="2">
+        <f>(G5-C5)/G5</f>
+        <v>-3.4812607689268575E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <f>(H5-D5)/H5</f>
+        <v>-4.6934033675289033E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1940</v>
+      </c>
+      <c r="C6" s="1">
+        <v>11.9619320796967</v>
+      </c>
+      <c r="D6" s="1">
+        <v>15.178854476675101</v>
+      </c>
+      <c r="F6">
+        <v>1940</v>
+      </c>
+      <c r="G6">
+        <v>12.65</v>
+      </c>
+      <c r="H6">
+        <v>15.17</v>
+      </c>
+      <c r="J6" s="2">
+        <f>(G6-C6)/G6</f>
+        <v>5.4392720972592921E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <f>(H6-D6)/H6</f>
+        <v>-5.8368336684908647E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1950</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.6733334278843692</v>
+      </c>
+      <c r="D7" s="1">
+        <v>11.461559356358901</v>
+      </c>
+      <c r="F7">
+        <v>1950</v>
+      </c>
+      <c r="G7">
+        <v>9.99</v>
+      </c>
+      <c r="H7">
+        <v>11.25</v>
+      </c>
+      <c r="J7" s="2">
+        <f>(G7-C7)/G7</f>
+        <v>3.1698355567130229E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <f>(H7-D7)/H7</f>
+        <v>-1.8805276120791189E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1960</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.5059995659363299</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10.379924458873999</v>
+      </c>
+      <c r="F8">
+        <v>1960</v>
+      </c>
+      <c r="G8">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="H8">
+        <v>10.59</v>
+      </c>
+      <c r="J8" s="2">
+        <f>(G8-C8)/G8</f>
+        <v>1.4368532336462443E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <f>(H8-D8)/H8</f>
+        <v>1.9837161579414606E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1970</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.7164162275907504</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10.4662567115308</v>
+      </c>
+      <c r="F9">
+        <v>1970</v>
+      </c>
+      <c r="G9">
+        <v>8.56</v>
+      </c>
+      <c r="H9">
+        <v>10.33</v>
+      </c>
+      <c r="J9" s="2">
+        <f>(G9-C9)/G9</f>
+        <v>-1.8272923783966111E-2</v>
+      </c>
+      <c r="K9" s="2">
+        <f>(H9-D9)/H9</f>
+        <v>-1.3190388337928363E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1980</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8.8914477934886094</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10.302733521904701</v>
+      </c>
+      <c r="F10">
+        <v>1980</v>
+      </c>
+      <c r="G10">
+        <v>8.81</v>
+      </c>
+      <c r="H10">
+        <v>10.18</v>
+      </c>
+      <c r="J10" s="2">
+        <f>(G10-C10)/G10</f>
+        <v>-9.2449254811133776E-3</v>
+      </c>
+      <c r="K10" s="2">
+        <f>(H10-D10)/H10</f>
+        <v>-1.2056338104587524E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1990</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9.0817992988698499</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9.9317506734395593</v>
+      </c>
+      <c r="F11">
+        <v>1990</v>
+      </c>
+      <c r="G11">
+        <v>9.01</v>
+      </c>
+      <c r="H11">
+        <v>9.83</v>
+      </c>
+      <c r="J11" s="2">
+        <f>(G11-C11)/G11</f>
+        <v>-7.9688456015371972E-3</v>
+      </c>
+      <c r="K11" s="2">
+        <f>(H11-D11)/H11</f>
+        <v>-1.0351034937900228E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>